<commit_message>
removed example results from policy review to make more clear this is just for demonstration purposes
</commit_message>
<xml_diff>
--- a/process/data/policy_review/_policy_review_template_v0_TO-BE-UPDATED.xlsx
+++ b/process/data/policy_review/_policy_review_template_v0_TO-BE-UPDATED.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/carl_higgs_rmit_edu_au/Documents/projects/global-indicators/process/data/policy_review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="11_72AD57B18700DA7EAFDA3711595ED87656CD08A1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED5D2F05-2BBD-4F4E-863A-F01332ED6F5C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F93F0DA7-1BA5-4FCF-BB1C-D6FBA22CE7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
   <si>
     <t>Weight</t>
   </si>
@@ -58,9 +58,6 @@
     <t>3a. Specific health-focused actions in national urban policy for the whole city</t>
   </si>
   <si>
-    <t>✓✓✗✓</t>
-  </si>
-  <si>
     <t>3b. Specific health-focused actions in subnational urban policy for the whole city</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
     <t xml:space="preserve">5a. Specific health-focused actions in national transport policy for the whole city </t>
   </si>
   <si>
-    <t>✗---</t>
-  </si>
-  <si>
     <t xml:space="preserve">5b. Specific health-focused actions in subnational transport policy for the whole city </t>
   </si>
   <si>
@@ -94,9 +88,6 @@
     <t>10. Requirements for distribution of employment</t>
   </si>
   <si>
-    <t>✓✓✓✓</t>
-  </si>
-  <si>
     <t>11. Requirements for ratio of jobs to housing</t>
   </si>
   <si>
@@ -118,15 +109,9 @@
     <t>17. Targets for walking participation</t>
   </si>
   <si>
-    <t>✓✓✓~</t>
-  </si>
-  <si>
     <t>18. Targets for cycling participation</t>
   </si>
   <si>
-    <t>✓✓✓✗</t>
-  </si>
-  <si>
     <t>19. Housing density requirements citywide or near transport or town centres</t>
   </si>
   <si>
@@ -146,6 +131,9 @@
   </si>
   <si>
     <t>Score</t>
+  </si>
+  <si>
+    <t>----</t>
   </si>
 </sst>
 </file>
@@ -222,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -247,6 +235,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -553,7 +544,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E3" sqref="E3:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,7 +593,7 @@
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -646,27 +637,15 @@
         <v>1</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="E5" s="4">
-        <v>1</v>
-      </c>
-      <c r="F5" s="4">
-        <v>1</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0</v>
-      </c>
-      <c r="H5" s="4">
-        <v>1</v>
-      </c>
-      <c r="I5" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="6">
         <v>0.5</v>
@@ -675,27 +654,15 @@
         <v>1</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="E6" s="4">
-        <v>1</v>
-      </c>
-      <c r="F6" s="4">
-        <v>1</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0</v>
-      </c>
-      <c r="H6" s="4">
-        <v>1</v>
-      </c>
-      <c r="I6" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="6">
         <v>0.5</v>
@@ -705,12 +672,12 @@
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="6">
         <v>0.5</v>
@@ -725,7 +692,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="6">
         <v>0.5</v>
@@ -734,18 +701,15 @@
         <v>1</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="E9" s="4">
-        <v>0</v>
-      </c>
-      <c r="I9" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" s="6">
         <v>0.5</v>
@@ -754,18 +718,15 @@
         <v>1</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="E10" s="4">
-        <v>0</v>
-      </c>
-      <c r="I10" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" s="6">
         <v>1</v>
@@ -775,12 +736,12 @@
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" s="6">
         <v>1</v>
@@ -789,18 +750,15 @@
         <v>1</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="E12" s="4">
-        <v>0</v>
-      </c>
-      <c r="I12" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13" s="6">
         <v>1</v>
@@ -809,18 +767,15 @@
         <v>1</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="E13" s="4">
-        <v>0</v>
-      </c>
-      <c r="I13" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B14" s="6">
         <v>1</v>
@@ -829,27 +784,15 @@
         <v>1</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="E14" s="4">
-        <v>1</v>
-      </c>
-      <c r="F14" s="4">
-        <v>1</v>
-      </c>
-      <c r="G14" s="4">
-        <v>0</v>
-      </c>
-      <c r="H14" s="4">
-        <v>1</v>
-      </c>
-      <c r="I14" s="6">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15" s="6">
         <v>1</v>
@@ -858,27 +801,15 @@
         <v>1</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="E15" s="4">
-        <v>1</v>
-      </c>
-      <c r="F15" s="4">
-        <v>1</v>
-      </c>
-      <c r="G15" s="4">
-        <v>1</v>
-      </c>
-      <c r="H15" s="4">
-        <v>1</v>
-      </c>
-      <c r="I15" s="6">
-        <v>3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B16" s="6">
         <v>1</v>
@@ -887,18 +818,15 @@
         <v>1</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="E16" s="4">
-        <v>0</v>
-      </c>
-      <c r="I16" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B17" s="6">
         <v>1</v>
@@ -907,18 +835,15 @@
         <v>1</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="E17" s="4">
-        <v>0</v>
-      </c>
-      <c r="I17" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B18" s="6">
         <v>1</v>
@@ -927,27 +852,15 @@
         <v>1</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="E18" s="4">
-        <v>1</v>
-      </c>
-      <c r="F18" s="4">
-        <v>1</v>
-      </c>
-      <c r="G18" s="4">
-        <v>1</v>
-      </c>
-      <c r="H18" s="4">
-        <v>1</v>
-      </c>
-      <c r="I18" s="6">
-        <v>3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B19" s="6">
         <v>1</v>
@@ -956,18 +869,15 @@
         <v>1</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="E19" s="4">
-        <v>0</v>
-      </c>
-      <c r="I19" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B20" s="6">
         <v>1</v>
@@ -976,27 +886,15 @@
         <v>1</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="E20" s="4">
-        <v>1</v>
-      </c>
-      <c r="F20" s="4">
-        <v>1</v>
-      </c>
-      <c r="G20" s="4">
-        <v>0</v>
-      </c>
-      <c r="H20" s="4">
-        <v>1</v>
-      </c>
-      <c r="I20" s="6">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B21" s="6">
         <v>1</v>
@@ -1005,27 +903,15 @@
         <v>1</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="E21" s="4">
-        <v>1</v>
-      </c>
-      <c r="F21" s="4">
-        <v>1</v>
-      </c>
-      <c r="G21" s="4">
-        <v>0</v>
-      </c>
-      <c r="H21" s="4">
-        <v>1</v>
-      </c>
-      <c r="I21" s="6">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B22" s="6">
         <v>1</v>
@@ -1033,28 +919,16 @@
       <c r="C22" s="6">
         <v>1</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>32</v>
+      <c r="D22" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="E22" s="4">
-        <v>1</v>
-      </c>
-      <c r="F22" s="4">
-        <v>1</v>
-      </c>
-      <c r="G22" s="4">
-        <v>1</v>
-      </c>
-      <c r="H22" s="4">
-        <v>-0.5</v>
-      </c>
-      <c r="I22" s="6">
-        <v>-1.5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B23" s="6">
         <v>1</v>
@@ -1063,27 +937,15 @@
         <v>1</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E23" s="4">
-        <v>1</v>
-      </c>
-      <c r="F23" s="4">
-        <v>1</v>
-      </c>
-      <c r="G23" s="4">
-        <v>1</v>
-      </c>
-      <c r="H23" s="4">
-        <v>-1</v>
-      </c>
-      <c r="I23" s="6">
-        <v>-3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B24" s="6">
         <v>1</v>
@@ -1092,27 +954,15 @@
         <v>1</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="E24" s="4">
-        <v>1</v>
-      </c>
-      <c r="F24" s="4">
-        <v>1</v>
-      </c>
-      <c r="G24" s="4">
-        <v>1</v>
-      </c>
-      <c r="H24" s="4">
-        <v>1</v>
-      </c>
-      <c r="I24" s="6">
-        <v>3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B25" s="6">
         <v>1</v>
@@ -1121,27 +971,15 @@
         <v>1</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="E25" s="4">
-        <v>1</v>
-      </c>
-      <c r="F25" s="4">
-        <v>1</v>
-      </c>
-      <c r="G25" s="4">
-        <v>1</v>
-      </c>
-      <c r="H25" s="4">
-        <v>1</v>
-      </c>
-      <c r="I25" s="6">
-        <v>3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B26" s="6">
         <v>1</v>
@@ -1150,27 +988,15 @@
         <v>1</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="E26" s="4">
-        <v>1</v>
-      </c>
-      <c r="F26" s="4">
-        <v>1</v>
-      </c>
-      <c r="G26" s="4">
-        <v>1</v>
-      </c>
-      <c r="H26" s="4">
-        <v>1</v>
-      </c>
-      <c r="I26" s="6">
-        <v>3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B27" s="6">
         <v>1</v>
@@ -1179,27 +1005,15 @@
         <v>1</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="E27" s="4">
-        <v>1</v>
-      </c>
-      <c r="F27" s="4">
-        <v>1</v>
-      </c>
-      <c r="G27" s="4">
-        <v>1</v>
-      </c>
-      <c r="H27" s="4">
-        <v>1</v>
-      </c>
-      <c r="I27" s="6">
-        <v>3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B28" s="6">
         <v>1</v>
@@ -1208,27 +1022,15 @@
         <v>1</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E28" s="4">
-        <v>1</v>
-      </c>
-      <c r="F28" s="4">
-        <v>1</v>
-      </c>
-      <c r="G28" s="4">
-        <v>1</v>
-      </c>
-      <c r="H28" s="4">
-        <v>-1</v>
-      </c>
-      <c r="I28" s="6">
-        <v>-3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B29" s="6">
         <v>1</v>
@@ -1238,21 +1040,21 @@
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E30" s="6">
-        <v>16.5</v>
+        <v>0</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6">
-        <v>18.5</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>